<commit_message>
whatever I have changed this excel file
</commit_message>
<xml_diff>
--- a/git-manual.xlsx
+++ b/git-manual.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>index,working tree都不会改变</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,6 +107,22 @@
   </si>
   <si>
     <t>git push &lt;remote-repo&gt; &lt;newbranch&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git merge origin/&lt;branchname&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将分支&lt;branchname&gt;与当前分支合并</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git cat-file -p [&lt;hash value&gt;]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看.git/objects/&lt;hash value前两位&gt;/路径下保存的对象文件的内容</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -451,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -556,6 +572,22 @@
       </c>
       <c r="B12" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
git diff v.s. git diff --cached
</commit_message>
<xml_diff>
--- a/git-manual.xlsx
+++ b/git-manual.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>index,working tree都不会改变</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -123,6 +123,22 @@
   </si>
   <si>
     <t>查看.git/objects/&lt;hash value前两位&gt;/路径下保存的对象文件的内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git diff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>比较working tree与index的差异</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git diff --cached HEAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>比较index与HEAD commit的差异</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -467,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -588,6 +604,22 @@
       </c>
       <c r="B14" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
git diff <commit1> <commit2>
</commit_message>
<xml_diff>
--- a/git-manual.xlsx
+++ b/git-manual.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>index,working tree都不会改变</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -139,6 +139,22 @@
   </si>
   <si>
     <t>比较index与HEAD commit的差异</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git diff --cached HEAD~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>比较index与HEAD~ commit的差异</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git diff HEAD~ HEAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>输出HEAD较之于HEAD~ commit的差异</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -483,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -620,6 +636,22 @@
       </c>
       <c r="B16" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>